<commit_message>
services py and bat file setup
</commit_message>
<xml_diff>
--- a/map/app_map.xlsx
+++ b/map/app_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CAST\code_\my-github-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CAST\code_\my-github-app\map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41771DB1-8E2B-4606-8CD0-51F53DEAD1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F2AABC-F073-44F3-8FC7-BA62F9B0CF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{46F8F908-AAEC-4096-BCF8-9C610F5D51ED}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,18 +56,9 @@
     <t>WebGoat_test</t>
   </si>
   <si>
-    <t>troux_id</t>
-  </si>
-  <si>
-    <t>gh_url</t>
-  </si>
-  <si>
     <t>app_name</t>
   </si>
   <si>
-    <t>hl_app_id</t>
-  </si>
-  <si>
     <t>7E876-899SUU</t>
   </si>
   <si>
@@ -76,6 +66,15 @@
   </si>
   <si>
     <t>7E876-777SUU</t>
+  </si>
+  <si>
+    <t>unique_id</t>
+  </si>
+  <si>
+    <t>github_url</t>
+  </si>
+  <si>
+    <t>highlight_app_id</t>
   </si>
 </sst>
 </file>
@@ -471,7 +470,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -479,21 +478,21 @@
     <col min="1" max="1" width="19.54296875" customWidth="1"/>
     <col min="2" max="2" width="30.7265625" customWidth="1"/>
     <col min="3" max="3" width="52.453125" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -501,7 +500,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -515,7 +514,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -529,7 +528,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
updated readme and map\app_map.xlsx
</commit_message>
<xml_diff>
--- a/map/app_map.xlsx
+++ b/map/app_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CAST\code_\my-github-app\map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F2AABC-F073-44F3-8FC7-BA62F9B0CF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADB71E4-6608-4710-8E21-7DA0C9176752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{46F8F908-AAEC-4096-BCF8-9C610F5D51ED}"/>
   </bookViews>
@@ -38,24 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>GitCloner</t>
-  </si>
-  <si>
-    <t>GitCloner1</t>
-  </si>
-  <si>
-    <t>https://github.com/hbe-cast/GitCloner</t>
-  </si>
-  <si>
-    <t>https://github.com/hbe-cast/GitCloner_1</t>
-  </si>
-  <si>
-    <t>https://github.com/hbe-cast/WebGoat_test</t>
-  </si>
-  <si>
-    <t>WebGoat_test</t>
-  </si>
-  <si>
     <t>app_name</t>
   </si>
   <si>
@@ -75,6 +57,24 @@
   </si>
   <si>
     <t>highlight_app_id</t>
+  </si>
+  <si>
+    <t>App1</t>
+  </si>
+  <si>
+    <t>App2</t>
+  </si>
+  <si>
+    <t>App3</t>
+  </si>
+  <si>
+    <t>https://github.com/user/app1</t>
+  </si>
+  <si>
+    <t>https://github.com/user/app2</t>
+  </si>
+  <si>
+    <t>https://github.com/user/app3</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,27 +483,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>358776</v>
@@ -511,37 +511,37 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D3">
-        <v>358777</v>
+        <v>358776</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>358778</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{76B7E272-AD47-40B7-B490-F44BFDF5C2DD}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{9DB49E27-5A86-45B4-82B8-0B776ED0BF12}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{3786ED6A-EE4E-4985-8F53-3C225F063A6D}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{763F9559-94D8-4759-9B17-C2D9D53DDA18}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{8160648C-B472-43A4-93DD-F657057C8E1A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>